<commit_message>
Keyword Driven Framework for Amazon
</commit_message>
<xml_diff>
--- a/src/main/resources/AmazonIndia.xlsx
+++ b/src/main/resources/AmazonIndia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prabh\IdeaProjects\AmazonIndiaKeywordDrivenFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DCD4C9-4D80-4E31-8A68-152BA5B25D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C98095-AB86-43BD-A6A6-CE53C70AF3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{4DF61A3E-747D-4F93-97C6-EFE4B3C1F08F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4DF61A3E-747D-4F93-97C6-EFE4B3C1F08F}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>locatorType</t>
   </si>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845169CE-15C9-4A6F-A86E-B4A132BC8515}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -702,10 +702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535E2B4E-CDA3-46B6-90A1-FB3271610127}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,161 +736,39 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{105FC490-7477-4893-92B4-CA58F414A01A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>